<commit_message>
update adsl spec to drop EOSDT
</commit_message>
<xml_diff>
--- a/pilot5-submission/pilot5-input/adamdata/adam-pilot-5.xlsx
+++ b/pilot5-submission/pilot5-input/adamdata/adam-pilot-5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccalmasini\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA3BBC6-528E-4E96-8ECD-FC2B7A5C301A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E04774-7E04-48BC-AD32-D7802EAC3F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="90" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="90" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Documents!$A$1:$C$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Methods!$A$1:$H$145</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ValueLevel!$A$1:$R$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$S$218</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$S$217</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5064" uniqueCount="1224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5057" uniqueCount="1222">
   <si>
     <t>Attribute</t>
   </si>
@@ -3705,12 +3705,6 @@
   </si>
   <si>
     <t>Set to DS.DSSTDTC if DSCAT == "DISPOSITION EVENT" and DSDECOD != "SCREEN FAILURE"</t>
-  </si>
-  <si>
-    <t>EOSDT</t>
-  </si>
-  <si>
-    <t>End of Study Date</t>
   </si>
   <si>
     <t>Adverse Event</t>
@@ -3828,7 +3822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3843,7 +3837,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -8335,11 +8328,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:S1001"/>
+  <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D194" sqref="D194"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C187" sqref="C187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -14174,7 +14167,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="177" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="2" t="s">
         <v>209</v>
       </c>
@@ -14208,7 +14201,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="2" t="s">
         <v>213</v>
       </c>
@@ -14242,7 +14235,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="2" t="s">
         <v>217</v>
       </c>
@@ -14273,7 +14266,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="2" t="s">
         <v>221</v>
       </c>
@@ -14306,7 +14299,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="181" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="2" t="s">
         <v>225</v>
       </c>
@@ -14340,7 +14333,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="182" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="2" t="s">
         <v>229</v>
       </c>
@@ -14374,7 +14367,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="2" t="s">
         <v>332</v>
       </c>
@@ -14407,7 +14400,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="2" t="s">
         <v>336</v>
       </c>
@@ -14438,7 +14431,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="2" t="s">
         <v>340</v>
       </c>
@@ -14469,7 +14462,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="2" t="s">
         <v>345</v>
       </c>
@@ -14500,7 +14493,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="2" t="s">
         <v>349</v>
       </c>
@@ -14533,7 +14526,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="2" t="s">
         <v>274</v>
       </c>
@@ -14567,7 +14560,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="2" t="s">
         <v>356</v>
       </c>
@@ -14598,120 +14591,120 @@
         <v>556</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A190" s="5">
-        <v>48</v>
-      </c>
-      <c r="B190" s="9" t="s">
+    <row r="190" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A190" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B190" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D190" s="9" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E190" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F190" s="5">
-        <v>8</v>
-      </c>
-      <c r="H190" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I190" s="2"/>
+        <v>557</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H190" s="5"/>
+      <c r="I190" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K190" s="2" t="s">
+        <v>559</v>
+      </c>
       <c r="L190" s="3"/>
       <c r="M190" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="O190" s="9" t="s">
-        <v>1211</v>
-      </c>
-    </row>
-    <row r="191" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O190" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="2" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="E191" s="2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>136</v>
+        <v>83</v>
       </c>
       <c r="H191" s="5"/>
       <c r="I191" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K191" s="2" t="s">
-        <v>559</v>
-      </c>
       <c r="L191" s="3"/>
       <c r="M191" s="2" t="s">
         <v>139</v>
       </c>
       <c r="O191" s="2" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="192" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="2" t="s">
-        <v>364</v>
+        <v>61</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>561</v>
+        <v>62</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>562</v>
+        <v>63</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H192" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="H192" s="6"/>
       <c r="I192" s="2" t="s">
         <v>27</v>
       </c>
       <c r="L192" s="3"/>
       <c r="M192" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="O192" s="2" t="s">
-        <v>563</v>
+        <v>59</v>
+      </c>
+      <c r="P192" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="193" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E193" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F193" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H193" s="6"/>
       <c r="I193" s="2" t="s">
@@ -14721,28 +14714,29 @@
       <c r="M193" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="O193" s="2"/>
       <c r="P193" s="2" t="s">
-        <v>66</v>
+        <v>466</v>
       </c>
     </row>
     <row r="194" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E194" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F194" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="H194" s="6"/>
       <c r="I194" s="2" t="s">
@@ -14752,29 +14746,28 @@
       <c r="M194" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O194" s="2"/>
       <c r="P194" s="2" t="s">
-        <v>466</v>
+        <v>78</v>
       </c>
     </row>
     <row r="195" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="E195" s="2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="F195" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="H195" s="6"/>
       <c r="I195" s="2" t="s">
@@ -14784,67 +14777,71 @@
       <c r="M195" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P195" s="2" t="s">
-        <v>78</v>
+      <c r="O195" s="2"/>
+      <c r="P195" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="196" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E196" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H196" s="6"/>
       <c r="I196" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="K196" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="L196" s="3"/>
       <c r="M196" s="2" t="s">
         <v>59</v>
       </c>
       <c r="O196" s="2"/>
       <c r="P196" t="s">
-        <v>399</v>
+        <v>107</v>
       </c>
     </row>
     <row r="197" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" s="2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E197" s="2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="F197" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H197" s="6"/>
       <c r="I197" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K197" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="L197" s="3"/>
       <c r="M197" s="2" t="s">
@@ -14852,34 +14849,34 @@
       </c>
       <c r="O197" s="2"/>
       <c r="P197" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="198" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E198" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F198" s="2" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="H198" s="6"/>
       <c r="I198" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K198" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="L198" s="3"/>
       <c r="M198" s="2" t="s">
@@ -14887,34 +14884,34 @@
       </c>
       <c r="O198" s="2"/>
       <c r="P198" t="s">
-        <v>110</v>
+        <v>400</v>
       </c>
     </row>
     <row r="199" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="F199" s="2" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="H199" s="6"/>
       <c r="I199" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K199" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="L199" s="3"/>
       <c r="M199" s="2" t="s">
@@ -14922,34 +14919,34 @@
       </c>
       <c r="O199" s="2"/>
       <c r="P199" t="s">
-        <v>400</v>
+        <v>118</v>
       </c>
     </row>
     <row r="200" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" s="2" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F200" s="2" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="H200" s="6"/>
       <c r="I200" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K200" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L200" s="3"/>
       <c r="M200" s="2" t="s">
@@ -14957,34 +14954,33 @@
       </c>
       <c r="O200" s="2"/>
       <c r="P200" t="s">
-        <v>118</v>
+        <v>401</v>
       </c>
     </row>
     <row r="201" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="F201" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H201" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="H201" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="I201" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="K201" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="L201" s="3"/>
       <c r="M201" s="2" t="s">
@@ -14992,21 +14988,21 @@
       </c>
       <c r="O201" s="2"/>
       <c r="P201" t="s">
-        <v>401</v>
+        <v>85</v>
       </c>
     </row>
     <row r="202" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="2" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E202" s="2" t="s">
         <v>82</v>
@@ -15026,21 +15022,21 @@
       </c>
       <c r="O202" s="2"/>
       <c r="P202" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="203" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>87</v>
+        <v>564</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>88</v>
+        <v>565</v>
       </c>
       <c r="E203" s="2" t="s">
         <v>82</v>
@@ -15048,9 +15044,7 @@
       <c r="F203" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H203" s="7" t="s">
-        <v>84</v>
-      </c>
+      <c r="H203" s="6"/>
       <c r="I203" s="2" t="s">
         <v>27</v>
       </c>
@@ -15060,53 +15054,56 @@
       </c>
       <c r="O203" s="2"/>
       <c r="P203" t="s">
-        <v>89</v>
+        <v>482</v>
       </c>
     </row>
     <row r="204" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" s="2" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>564</v>
+        <v>91</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>565</v>
+        <v>92</v>
       </c>
       <c r="E204" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F204" s="2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="H204" s="6"/>
       <c r="I204" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="K204" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="L204" s="3"/>
       <c r="M204" s="2" t="s">
         <v>59</v>
       </c>
       <c r="O204" s="2"/>
       <c r="P204" t="s">
-        <v>482</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="205" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>91</v>
+        <v>234</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>92</v>
+        <v>235</v>
       </c>
       <c r="E205" s="2" t="s">
         <v>64</v>
@@ -15127,34 +15124,34 @@
       </c>
       <c r="O205" s="2"/>
       <c r="P205" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="206" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E206" s="2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="F206" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H206" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="H206" s="7"/>
       <c r="I206" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K206" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="L206" s="3"/>
       <c r="M206" s="2" t="s">
@@ -15162,124 +15159,120 @@
       </c>
       <c r="O206" s="2"/>
       <c r="P206" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="207" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>237</v>
+        <v>163</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>238</v>
+        <v>164</v>
       </c>
       <c r="E207" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F207" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H207" s="7"/>
+        <v>165</v>
+      </c>
+      <c r="H207" s="6"/>
       <c r="I207" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K207" s="2" t="s">
-        <v>98</v>
+        <v>566</v>
       </c>
       <c r="L207" s="3"/>
       <c r="M207" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O207" s="2"/>
-      <c r="P207" t="s">
-        <v>1209</v>
+        <v>139</v>
+      </c>
+      <c r="O207" s="2" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="208" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="E208" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F208" s="2" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="H208" s="6"/>
       <c r="I208" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K208" s="2" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="L208" s="3"/>
       <c r="M208" s="2" t="s">
         <v>139</v>
       </c>
       <c r="O208" s="2" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="209" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="E209" s="2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="F209" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H209" s="6"/>
+      <c r="H209" s="7"/>
       <c r="I209" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="K209" s="2" t="s">
-        <v>568</v>
       </c>
       <c r="L209" s="3"/>
       <c r="M209" s="2" t="s">
         <v>139</v>
       </c>
       <c r="O209" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="210" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>179</v>
+        <v>571</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>180</v>
+        <v>572</v>
       </c>
       <c r="E210" s="2" t="s">
         <v>82</v>
@@ -15287,7 +15280,9 @@
       <c r="F210" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H210" s="7"/>
+      <c r="H210" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="I210" s="2" t="s">
         <v>27</v>
       </c>
@@ -15296,21 +15291,21 @@
         <v>139</v>
       </c>
       <c r="O210" s="2" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
     </row>
     <row r="211" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="2" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>571</v>
+        <v>159</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>572</v>
+        <v>160</v>
       </c>
       <c r="E211" s="2" t="s">
         <v>82</v>
@@ -15329,21 +15324,21 @@
         <v>139</v>
       </c>
       <c r="O211" s="2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="212" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="2" t="s">
-        <v>93</v>
+        <v>149</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>159</v>
+        <v>575</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>160</v>
+        <v>576</v>
       </c>
       <c r="E212" s="2" t="s">
         <v>82</v>
@@ -15351,72 +15346,70 @@
       <c r="F212" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H212" s="7" t="s">
-        <v>84</v>
-      </c>
+      <c r="H212" s="7"/>
       <c r="I212" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="K212" s="2" t="s">
+        <v>577</v>
       </c>
       <c r="L212" s="3"/>
       <c r="M212" s="2" t="s">
         <v>139</v>
       </c>
       <c r="O212" s="2" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
     </row>
     <row r="213" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" s="2" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="E213" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F213" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H213" s="7"/>
+        <v>168</v>
+      </c>
+      <c r="H213" s="6"/>
       <c r="I213" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="K213" s="2" t="s">
-        <v>577</v>
       </c>
       <c r="L213" s="3"/>
       <c r="M213" s="2" t="s">
         <v>139</v>
       </c>
       <c r="O213" s="2" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
     </row>
     <row r="214" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="E214" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F214" s="2" t="s">
-        <v>168</v>
+        <v>75</v>
       </c>
       <c r="H214" s="6"/>
       <c r="I214" s="2" t="s">
@@ -15427,27 +15420,27 @@
         <v>139</v>
       </c>
       <c r="O214" s="2" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="215" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="E215" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F215" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="H215" s="6"/>
       <c r="I215" s="2" t="s">
@@ -15458,29 +15451,29 @@
         <v>139</v>
       </c>
       <c r="O215" s="2" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
     <row r="216" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="E216" s="2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="F216" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H216" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="H216" s="7"/>
       <c r="I216" s="2" t="s">
         <v>27</v>
       </c>
@@ -15489,74 +15482,46 @@
         <v>139</v>
       </c>
       <c r="O216" s="2" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="217" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>588</v>
+        <v>246</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>589</v>
+        <v>247</v>
       </c>
       <c r="E217" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F217" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H217" s="7"/>
+        <v>61</v>
+      </c>
+      <c r="H217" s="6"/>
       <c r="I217" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="K217" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="L217" s="3"/>
       <c r="M217" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="O217" s="2" t="s">
-        <v>590</v>
+        <v>59</v>
+      </c>
+      <c r="O217" s="2"/>
+      <c r="P217" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="218" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A218" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D218" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E218" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F218" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H218" s="6"/>
-      <c r="I218" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K218" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="L218" s="3"/>
-      <c r="M218" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O218" s="2"/>
-      <c r="P218" t="s">
-        <v>495</v>
-      </c>
+      <c r="H218" s="5"/>
     </row>
     <row r="219" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H219" s="5"/>
@@ -15583,10 +15548,10 @@
       <c r="H226" s="5"/>
     </row>
     <row r="227" spans="7:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G227" s="2"/>
       <c r="H227" s="5"/>
     </row>
     <row r="228" spans="7:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G228" s="2"/>
       <c r="H228" s="5"/>
     </row>
     <row r="229" spans="7:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17905,11 +17870,8 @@
     <row r="1000" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H1000" s="5"/>
     </row>
-    <row r="1001" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H1001" s="5"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:S218" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:S217" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -19516,7 +19478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -20964,13 +20926,13 @@
       <c r="E71" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F71" s="11" t="s">
-        <v>1216</v>
+      <c r="F71" s="10" t="s">
+        <v>1214</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="I71" s="11"/>
+      <c r="I71" s="10"/>
     </row>
     <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
@@ -20985,8 +20947,8 @@
       <c r="E72" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F72" s="11" t="s">
-        <v>1217</v>
+      <c r="F72" s="10" t="s">
+        <v>1215</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>681</v>
@@ -21026,13 +20988,13 @@
       <c r="E74" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F74" s="11" t="s">
-        <v>1218</v>
+      <c r="F74" s="10" t="s">
+        <v>1216</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="I74" s="11"/>
+      <c r="I74" s="10"/>
     </row>
     <row r="75" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
@@ -21047,13 +21009,13 @@
       <c r="E75" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F75" s="11" t="s">
-        <v>1223</v>
+      <c r="F75" s="10" t="s">
+        <v>1221</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>683</v>
       </c>
-      <c r="I75" s="11"/>
+      <c r="I75" s="10"/>
     </row>
     <row r="76" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
@@ -21068,13 +21030,13 @@
       <c r="E76" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F76" s="11" t="s">
-        <v>1219</v>
+      <c r="F76" s="10" t="s">
+        <v>1217</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>686</v>
       </c>
-      <c r="I76" s="11"/>
+      <c r="I76" s="10"/>
     </row>
     <row r="77" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
@@ -21089,13 +21051,13 @@
       <c r="E77" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F77" s="11" t="s">
-        <v>1220</v>
+      <c r="F77" s="10" t="s">
+        <v>1218</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="I77" s="11"/>
+      <c r="I77" s="10"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
@@ -21110,13 +21072,13 @@
       <c r="E78" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F78" s="11" t="s">
-        <v>1221</v>
+      <c r="F78" s="10" t="s">
+        <v>1219</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="I78" s="11"/>
+      <c r="I78" s="10"/>
     </row>
     <row r="79" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
@@ -21131,8 +21093,8 @@
       <c r="E79" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F79" s="11" t="s">
-        <v>1222</v>
+      <c r="F79" s="10" t="s">
+        <v>1220</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>684</v>

</xml_diff>

<commit_message>
conversion programs quieted and using decimal_as_floats=TRUE; rerun of all datasets and tlfs;  placeholder section for ADRG
</commit_message>
<xml_diff>
--- a/pilot5-submission/pilot5-input/adamdata/adam-pilot-5.xlsx
+++ b/pilot5-submission/pilot5-input/adamdata/adam-pilot-5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cp903461\Downloads\datasetJSON Pilot 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bs832471\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B7D320-95C3-48CA-8A87-AB3E1A927A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF11C82C-F6EF-413B-89BD-15DA31EDCD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ValueLevel!$A$1:$R$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$S$217</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5057" uniqueCount="1222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5055" uniqueCount="1223">
   <si>
     <t>Attribute</t>
   </si>
@@ -3729,17 +3729,34 @@
   </si>
   <si>
     <t>StandardVersion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3815,20 +3832,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -8338,9 +8359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L75" sqref="L75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9304,12 +9325,10 @@
       <c r="E28" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="F28" s="5">
+        <v>8</v>
+      </c>
+      <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="2" t="s">
         <v>27</v>
@@ -9336,11 +9355,12 @@
         <v>184</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="G29" s="10"/>
       <c r="H29" s="5"/>
       <c r="I29" s="2" t="s">
         <v>27</v>
@@ -9367,11 +9387,12 @@
         <v>188</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="G30" s="10"/>
       <c r="H30" s="5"/>
       <c r="I30" s="2" t="s">
         <v>27</v>
@@ -9398,7 +9419,7 @@
         <v>192</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>83</v>
@@ -17890,7 +17911,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17984,14 +18005,14 @@
       <c r="E2" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>115</v>
+      <c r="G2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>27</v>
@@ -18019,14 +18040,14 @@
       <c r="E3" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>115</v>
+      <c r="G3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>27</v>
@@ -18054,14 +18075,14 @@
       <c r="E4" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>115</v>
+      <c r="G4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>27</v>
@@ -18089,14 +18110,14 @@
       <c r="E5" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>115</v>
+      <c r="G5" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>27</v>
@@ -18124,14 +18145,14 @@
       <c r="E6" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>115</v>
+      <c r="G6" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>27</v>
@@ -18159,14 +18180,14 @@
       <c r="E7" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>115</v>
+      <c r="G7" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>27</v>
@@ -18194,14 +18215,14 @@
       <c r="E8" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>115</v>
+      <c r="G8" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>27</v>
@@ -18229,14 +18250,14 @@
       <c r="E9" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>115</v>
+      <c r="G9" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>27</v>
@@ -18264,14 +18285,14 @@
       <c r="E10" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>115</v>
+      <c r="G10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>27</v>
@@ -18299,14 +18320,14 @@
       <c r="E11" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>115</v>
+      <c r="G11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>27</v>
@@ -18334,14 +18355,14 @@
       <c r="E12" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>115</v>
+      <c r="G12" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>27</v>
@@ -18369,14 +18390,14 @@
       <c r="E13" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>115</v>
+      <c r="G13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>27</v>
@@ -18404,14 +18425,14 @@
       <c r="E14" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>115</v>
+      <c r="G14" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>27</v>
@@ -18439,14 +18460,14 @@
       <c r="E15" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>115</v>
+      <c r="G15" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>27</v>
@@ -18474,14 +18495,14 @@
       <c r="E16" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>115</v>
+      <c r="G16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>27</v>
@@ -19485,7 +19506,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F74" sqref="F74"/>
@@ -28139,7 +28160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
     </sheetView>

</xml_diff>

<commit_message>
Closes #111 update adrg to mention the json standard version dataset json v110 from cdisc (#123)
* remove diffdf from lock file; more breakdown of installing packages in adrg.

* remove pilot3 adrg images

* conversion programs quieted and using decimal_as_floats=TRUE; rerun of all datasets and tlfs;  placeholder section for ADRG

* chore: styling

* using v5 in xpt calls now.  1.1 and 1.0 comparisions.  conformance summaries provided

* inserted pilot3 findings into ADRG
</commit_message>
<xml_diff>
--- a/pilot5-submission/pilot5-input/adamdata/adam-pilot-5.xlsx
+++ b/pilot5-submission/pilot5-input/adamdata/adam-pilot-5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cp903461\Downloads\datasetJSON Pilot 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bs832471\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B7D320-95C3-48CA-8A87-AB3E1A927A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF11C82C-F6EF-413B-89BD-15DA31EDCD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ValueLevel!$A$1:$R$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$S$217</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5057" uniqueCount="1222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5055" uniqueCount="1223">
   <si>
     <t>Attribute</t>
   </si>
@@ -3729,17 +3729,34 @@
   </si>
   <si>
     <t>StandardVersion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3815,20 +3832,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -8338,9 +8359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L75" sqref="L75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9304,12 +9325,10 @@
       <c r="E28" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="F28" s="5">
+        <v>8</v>
+      </c>
+      <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="2" t="s">
         <v>27</v>
@@ -9336,11 +9355,12 @@
         <v>184</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="G29" s="10"/>
       <c r="H29" s="5"/>
       <c r="I29" s="2" t="s">
         <v>27</v>
@@ -9367,11 +9387,12 @@
         <v>188</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="G30" s="10"/>
       <c r="H30" s="5"/>
       <c r="I30" s="2" t="s">
         <v>27</v>
@@ -9398,7 +9419,7 @@
         <v>192</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>83</v>
@@ -17890,7 +17911,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17984,14 +18005,14 @@
       <c r="E2" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>115</v>
+      <c r="G2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>27</v>
@@ -18019,14 +18040,14 @@
       <c r="E3" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>115</v>
+      <c r="G3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>27</v>
@@ -18054,14 +18075,14 @@
       <c r="E4" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>115</v>
+      <c r="G4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>27</v>
@@ -18089,14 +18110,14 @@
       <c r="E5" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>115</v>
+      <c r="G5" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>27</v>
@@ -18124,14 +18145,14 @@
       <c r="E6" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>115</v>
+      <c r="G6" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>27</v>
@@ -18159,14 +18180,14 @@
       <c r="E7" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>115</v>
+      <c r="G7" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>27</v>
@@ -18194,14 +18215,14 @@
       <c r="E8" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>115</v>
+      <c r="G8" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>27</v>
@@ -18229,14 +18250,14 @@
       <c r="E9" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>115</v>
+      <c r="G9" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>27</v>
@@ -18264,14 +18285,14 @@
       <c r="E10" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>115</v>
+      <c r="G10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>27</v>
@@ -18299,14 +18320,14 @@
       <c r="E11" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>115</v>
+      <c r="G11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>27</v>
@@ -18334,14 +18355,14 @@
       <c r="E12" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>115</v>
+      <c r="G12" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>27</v>
@@ -18369,14 +18390,14 @@
       <c r="E13" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>115</v>
+      <c r="G13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>27</v>
@@ -18404,14 +18425,14 @@
       <c r="E14" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>115</v>
+      <c r="G14" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>27</v>
@@ -18439,14 +18460,14 @@
       <c r="E15" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>115</v>
+      <c r="G15" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>27</v>
@@ -18474,14 +18495,14 @@
       <c r="E16" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>115</v>
+      <c r="G16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>27</v>
@@ -19485,7 +19506,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F74" sqref="F74"/>
@@ -28139,7 +28160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
     </sheetView>

</xml_diff>